<commit_message>
simulator runs. need to test
</commit_message>
<xml_diff>
--- a/raw-data/scenarios.xlsx
+++ b/raw-data/scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n8tha\Documents\R\multimcm-simulationstudy\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBECFBC-ABC1-4D00-8F5C-00540B2C56C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BA0139-1A21-4055-A4B1-F2497F0F9933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9DDBCAF9-FF84-4D35-9E45-B096DB59D2E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>list(list(shape=1,scale=1),list(shape=1,scale=1),list(shape=1,scale=1))</t>
+  </si>
+  <si>
+    <t>list(list(shape=2,scale=1),list(shape=1,scale=1),list(shape=1,scale=2))</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +561,7 @@
         <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L2" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
check arguments make sense, right way round etc
</commit_message>
<xml_diff>
--- a/raw-data/scenarios.xlsx
+++ b/raw-data/scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n8tha\Documents\R\multimcm-simulationstudy\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BA0139-1A21-4055-A4B1-F2497F0F9933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09554520-F799-4A74-BD29-E274440163AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9DDBCAF9-FF84-4D35-9E45-B096DB59D2E0}"/>
+    <workbookView xWindow="4430" yWindow="1200" windowWidth="14400" windowHeight="8710" xr2:uid="{9DDBCAF9-FF84-4D35-9E45-B096DB59D2E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,26 +472,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B56317-D8BB-4F0B-ADA1-CFA230DEFB8B}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26:E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" customWidth="1"/>
-    <col min="12" max="12" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.81640625" customWidth="1"/>
+    <col min="12" max="12" width="27.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -529,7 +529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -543,13 +543,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
       </c>
       <c r="G2">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H2">
         <v>5</v>
@@ -567,7 +567,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -581,13 +581,13 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
       <c r="G3">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H3">
         <v>5</v>
@@ -605,7 +605,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -619,13 +619,13 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
       <c r="G4">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H4">
         <v>5</v>
@@ -643,7 +643,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -657,13 +657,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
       </c>
       <c r="G5">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H5">
         <v>5</v>
@@ -681,7 +681,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -695,13 +695,13 @@
         <v>50</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
       </c>
       <c r="G6">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H6">
         <v>5</v>
@@ -719,7 +719,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -733,13 +733,13 @@
         <v>50</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
       <c r="G7">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H7">
         <v>5</v>
@@ -757,7 +757,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -771,13 +771,13 @@
         <v>50</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
       </c>
       <c r="G8">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H8">
         <v>5</v>
@@ -795,7 +795,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -809,13 +809,13 @@
         <v>50</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
       </c>
       <c r="G9">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H9">
         <v>5</v>
@@ -833,7 +833,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -847,13 +847,13 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
       </c>
       <c r="G10">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H10">
         <v>5</v>
@@ -871,7 +871,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -885,13 +885,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
       </c>
       <c r="G11">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H11">
         <v>5</v>
@@ -909,7 +909,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -923,13 +923,13 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F12" t="s">
         <v>9</v>
       </c>
       <c r="G12">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H12">
         <v>5</v>
@@ -947,7 +947,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -961,13 +961,13 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
       </c>
       <c r="G13">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H13">
         <v>5</v>
@@ -985,7 +985,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -999,13 +999,13 @@
         <v>50</v>
       </c>
       <c r="E14">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F14" t="s">
         <v>9</v>
       </c>
       <c r="G14">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H14">
         <v>5</v>
@@ -1023,7 +1023,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1037,13 +1037,13 @@
         <v>50</v>
       </c>
       <c r="E15">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F15" t="s">
         <v>9</v>
       </c>
       <c r="G15">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H15">
         <v>5</v>
@@ -1061,7 +1061,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1075,13 +1075,13 @@
         <v>50</v>
       </c>
       <c r="E16">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F16" t="s">
         <v>9</v>
       </c>
       <c r="G16">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H16">
         <v>5</v>
@@ -1099,7 +1099,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1113,13 +1113,13 @@
         <v>50</v>
       </c>
       <c r="E17">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F17" t="s">
         <v>9</v>
       </c>
       <c r="G17">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H17">
         <v>5</v>
@@ -1137,7 +1137,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1151,13 +1151,13 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
       </c>
       <c r="G18">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H18">
         <v>5</v>
@@ -1175,7 +1175,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1189,13 +1189,13 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
       </c>
       <c r="G19">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H19">
         <v>5</v>
@@ -1213,7 +1213,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1227,13 +1227,13 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F20" t="s">
         <v>10</v>
       </c>
       <c r="G20">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H20">
         <v>5</v>
@@ -1251,7 +1251,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1265,13 +1265,13 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F21" t="s">
         <v>10</v>
       </c>
       <c r="G21">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H21">
         <v>5</v>
@@ -1289,7 +1289,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1303,13 +1303,13 @@
         <v>50</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F22" t="s">
         <v>10</v>
       </c>
       <c r="G22">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H22">
         <v>5</v>
@@ -1327,7 +1327,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1341,13 +1341,13 @@
         <v>50</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F23" t="s">
         <v>10</v>
       </c>
       <c r="G23">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H23">
         <v>5</v>
@@ -1365,7 +1365,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1379,13 +1379,13 @@
         <v>50</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F24" t="s">
         <v>10</v>
       </c>
       <c r="G24">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H24">
         <v>5</v>
@@ -1403,7 +1403,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1417,13 +1417,13 @@
         <v>50</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F25" t="s">
         <v>10</v>
       </c>
       <c r="G25">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H25">
         <v>5</v>
@@ -1441,7 +1441,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1455,13 +1455,13 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F26" t="s">
         <v>10</v>
       </c>
       <c r="G26">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H26">
         <v>5</v>
@@ -1479,7 +1479,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1493,13 +1493,13 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F27" t="s">
         <v>10</v>
       </c>
       <c r="G27">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H27">
         <v>5</v>
@@ -1517,7 +1517,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1531,13 +1531,13 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F28" t="s">
         <v>10</v>
       </c>
       <c r="G28">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H28">
         <v>5</v>
@@ -1555,7 +1555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1569,13 +1569,13 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F29" t="s">
         <v>10</v>
       </c>
       <c r="G29">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H29">
         <v>5</v>
@@ -1593,7 +1593,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1607,13 +1607,13 @@
         <v>50</v>
       </c>
       <c r="E30">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F30" t="s">
         <v>10</v>
       </c>
       <c r="G30">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H30">
         <v>5</v>
@@ -1631,7 +1631,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1645,13 +1645,13 @@
         <v>50</v>
       </c>
       <c r="E31">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F31" t="s">
         <v>10</v>
       </c>
       <c r="G31">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H31">
         <v>5</v>
@@ -1669,7 +1669,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1683,13 +1683,13 @@
         <v>50</v>
       </c>
       <c r="E32">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F32" t="s">
         <v>10</v>
       </c>
       <c r="G32">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H32">
         <v>5</v>
@@ -1707,7 +1707,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1721,13 +1721,13 @@
         <v>50</v>
       </c>
       <c r="E33">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="F33" t="s">
         <v>10</v>
       </c>
       <c r="G33">
-        <v>0.2</v>
+        <v>-1.39</v>
       </c>
       <c r="H33">
         <v>5</v>

</xml_diff>

<commit_message>
modified input scenario data
</commit_message>
<xml_diff>
--- a/raw-data/scenarios.xlsx
+++ b/raw-data/scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n8tha\Documents\R\multimcm-simulationstudy\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB98D39-F6DE-48D4-9464-4F5DB37AD99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72D3A95-F983-437C-A9BA-16B12C56A54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14355" yWindow="1995" windowWidth="14175" windowHeight="13860" xr2:uid="{9DDBCAF9-FF84-4D35-9E45-B096DB59D2E0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9DDBCAF9-FF84-4D35-9E45-B096DB59D2E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>weibull</t>
   </si>
   <si>
-    <t>list(list(shape=1,scale=1))</t>
-  </si>
-  <si>
     <t>data_id</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>sigma_sd_cf_prior</t>
+  </si>
+  <si>
+    <t>list(list(shape=1,scale=1),list(shape=1,scale=0.1))</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="P2" sqref="P2:P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +488,7 @@
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" customWidth="1"/>
@@ -496,16 +496,16 @@
     <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -523,19 +523,19 @@
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>4</v>
@@ -600,7 +600,7 @@
         <v>11</v>
       </c>
       <c r="P2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q2" t="s">
         <v>10</v>
@@ -653,7 +653,7 @@
         <v>11</v>
       </c>
       <c r="P3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q3" t="s">
         <v>10</v>
@@ -706,7 +706,7 @@
         <v>11</v>
       </c>
       <c r="P4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q4" t="s">
         <v>10</v>
@@ -759,7 +759,7 @@
         <v>11</v>
       </c>
       <c r="P5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q5" t="s">
         <v>10</v>
@@ -812,7 +812,7 @@
         <v>11</v>
       </c>
       <c r="P6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q6" t="s">
         <v>10</v>
@@ -865,7 +865,7 @@
         <v>11</v>
       </c>
       <c r="P7" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q7" t="s">
         <v>10</v>
@@ -918,7 +918,7 @@
         <v>11</v>
       </c>
       <c r="P8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q8" t="s">
         <v>10</v>
@@ -971,7 +971,7 @@
         <v>11</v>
       </c>
       <c r="P9" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q9" t="s">
         <v>10</v>
@@ -997,10 +997,10 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H10">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I10">
         <v>2.5</v>
@@ -1024,7 +1024,7 @@
         <v>11</v>
       </c>
       <c r="P10" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q10" t="s">
         <v>10</v>
@@ -1050,10 +1050,10 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H11">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I11">
         <v>2.5</v>
@@ -1077,7 +1077,7 @@
         <v>11</v>
       </c>
       <c r="P11" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q11" t="s">
         <v>10</v>
@@ -1103,10 +1103,10 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H12">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I12">
         <v>2.5</v>
@@ -1130,7 +1130,7 @@
         <v>11</v>
       </c>
       <c r="P12" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q12" t="s">
         <v>10</v>
@@ -1156,10 +1156,10 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I13">
         <v>2.5</v>
@@ -1183,7 +1183,7 @@
         <v>11</v>
       </c>
       <c r="P13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q13" t="s">
         <v>10</v>
@@ -1209,10 +1209,10 @@
         <v>0.5</v>
       </c>
       <c r="G14">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H14">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I14">
         <v>2.5</v>
@@ -1236,7 +1236,7 @@
         <v>11</v>
       </c>
       <c r="P14" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q14" t="s">
         <v>10</v>
@@ -1262,10 +1262,10 @@
         <v>0.5</v>
       </c>
       <c r="G15">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H15">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I15">
         <v>2.5</v>
@@ -1289,7 +1289,7 @@
         <v>11</v>
       </c>
       <c r="P15" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q15" t="s">
         <v>10</v>
@@ -1315,10 +1315,10 @@
         <v>0.5</v>
       </c>
       <c r="G16">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H16">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I16">
         <v>2.5</v>
@@ -1342,7 +1342,7 @@
         <v>11</v>
       </c>
       <c r="P16" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q16" t="s">
         <v>10</v>
@@ -1368,10 +1368,10 @@
         <v>0.5</v>
       </c>
       <c r="G17">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H17">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I17">
         <v>2.5</v>
@@ -1395,7 +1395,7 @@
         <v>11</v>
       </c>
       <c r="P17" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q17" t="s">
         <v>10</v>
@@ -1448,7 +1448,7 @@
         <v>11</v>
       </c>
       <c r="P18" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q18" t="s">
         <v>10</v>
@@ -1501,7 +1501,7 @@
         <v>11</v>
       </c>
       <c r="P19" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q19" t="s">
         <v>10</v>
@@ -1554,7 +1554,7 @@
         <v>11</v>
       </c>
       <c r="P20" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q20" t="s">
         <v>10</v>
@@ -1607,7 +1607,7 @@
         <v>11</v>
       </c>
       <c r="P21" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q21" t="s">
         <v>10</v>
@@ -1660,7 +1660,7 @@
         <v>11</v>
       </c>
       <c r="P22" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q22" t="s">
         <v>10</v>
@@ -1713,7 +1713,7 @@
         <v>11</v>
       </c>
       <c r="P23" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q23" t="s">
         <v>10</v>
@@ -1766,7 +1766,7 @@
         <v>11</v>
       </c>
       <c r="P24" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q24" t="s">
         <v>10</v>
@@ -1819,7 +1819,7 @@
         <v>11</v>
       </c>
       <c r="P25" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q25" t="s">
         <v>10</v>
@@ -1845,10 +1845,10 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H26">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I26">
         <v>2.5</v>
@@ -1872,7 +1872,7 @@
         <v>11</v>
       </c>
       <c r="P26" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q26" t="s">
         <v>10</v>
@@ -1898,10 +1898,10 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H27">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I27">
         <v>2.5</v>
@@ -1925,7 +1925,7 @@
         <v>11</v>
       </c>
       <c r="P27" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q27" t="s">
         <v>10</v>
@@ -1951,10 +1951,10 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H28">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I28">
         <v>2.5</v>
@@ -1978,7 +1978,7 @@
         <v>11</v>
       </c>
       <c r="P28" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q28" t="s">
         <v>10</v>
@@ -2004,10 +2004,10 @@
         <v>0</v>
       </c>
       <c r="G29">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H29">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I29">
         <v>2.5</v>
@@ -2031,7 +2031,7 @@
         <v>11</v>
       </c>
       <c r="P29" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q29" t="s">
         <v>10</v>
@@ -2057,10 +2057,10 @@
         <v>0.5</v>
       </c>
       <c r="G30">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H30">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I30">
         <v>2.5</v>
@@ -2084,7 +2084,7 @@
         <v>11</v>
       </c>
       <c r="P30" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q30" t="s">
         <v>10</v>
@@ -2110,10 +2110,10 @@
         <v>0.5</v>
       </c>
       <c r="G31">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H31">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I31">
         <v>2.5</v>
@@ -2137,7 +2137,7 @@
         <v>11</v>
       </c>
       <c r="P31" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q31" t="s">
         <v>10</v>
@@ -2163,10 +2163,10 @@
         <v>0.5</v>
       </c>
       <c r="G32">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H32">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I32">
         <v>2.5</v>
@@ -2190,7 +2190,7 @@
         <v>11</v>
       </c>
       <c r="P32" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q32" t="s">
         <v>10</v>
@@ -2216,10 +2216,10 @@
         <v>0.5</v>
       </c>
       <c r="G33">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H33">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="I33">
         <v>2.5</v>
@@ -2243,7 +2243,7 @@
         <v>11</v>
       </c>
       <c r="P33" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q33" t="s">
         <v>10</v>

</xml_diff>